<commit_message>
Block Global Client Changes
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="CHN_SIT_FullCycle" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="105">
   <si>
     <t>Description</t>
   </si>
@@ -349,10 +349,10 @@
     <t>critical</t>
   </si>
   <si>
-    <t>AmendGlobalClient</t>
-  </si>
-  <si>
-    <t>Change Details in Created Global Client</t>
+    <t>BlockGlobalVendor</t>
+  </si>
+  <si>
+    <t>Block Created Global Vendor</t>
   </si>
 </sst>
 </file>
@@ -771,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,27 +829,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -857,13 +857,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -871,13 +871,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -885,13 +885,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>26</v>
@@ -913,13 +913,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -927,13 +927,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -941,13 +941,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -955,13 +955,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -969,15 +969,323 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -989,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,27 +1355,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -1075,13 +1383,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -1089,13 +1397,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -1103,13 +1411,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -1117,7 +1425,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>26</v>
@@ -1131,13 +1439,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -1145,13 +1453,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -1159,13 +1467,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -1173,13 +1481,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -1187,15 +1495,323 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1207,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,27 +1854,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -1266,13 +1882,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -1280,27 +1896,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -1308,41 +1924,41 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -1350,41 +1966,41 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -1392,13 +2008,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -1406,30 +2022,324 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1443,10 +2353,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B14"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,13 +2383,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -1487,13 +2397,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -1501,41 +2411,41 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -1543,41 +2453,41 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -1585,41 +2495,41 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -1627,13 +2537,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -1641,16 +2551,324 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1833,10 +3051,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,27 +3109,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -1919,13 +3137,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -1933,13 +3151,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -1947,13 +3165,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -1961,7 +3179,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>26</v>
@@ -1975,13 +3193,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -1989,13 +3207,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -2003,13 +3221,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -2017,13 +3235,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -2031,15 +3249,323 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2051,10 +3577,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,27 +3635,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -2137,13 +3663,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -2151,13 +3677,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -2165,13 +3691,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -2179,7 +3705,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>26</v>
@@ -2193,13 +3719,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -2207,13 +3733,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -2221,13 +3747,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -2235,13 +3761,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -2249,15 +3775,323 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2361,10 +4195,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,7 +4234,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2428,7 +4262,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2442,7 +4276,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2470,7 +4304,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2484,7 +4318,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2512,7 +4346,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2526,7 +4360,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2568,7 +4402,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2582,7 +4416,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2610,7 +4444,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2624,7 +4458,7 @@
         <v>63</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2652,7 +4486,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2666,7 +4500,7 @@
         <v>74</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2680,7 +4514,7 @@
         <v>76</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2694,7 +4528,7 @@
         <v>70</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2708,7 +4542,7 @@
         <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2722,7 +4556,7 @@
         <v>55</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2736,7 +4570,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2750,7 +4584,7 @@
         <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2835,6 +4669,48 @@
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Block Company Client,Brand,Product Changes
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="CHN_SIT_FullCycle" sheetId="6" r:id="rId1"/>
@@ -800,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -3956,8 +3956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3984,13 +3984,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -3998,58 +3998,58 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4063,35 +4063,35 @@
         <v>99</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4385,7 +4385,7 @@
         <v>76</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4455,7 +4455,7 @@
         <v>67</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4469,7 +4469,7 @@
         <v>45</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4483,7 +4483,7 @@
         <v>46</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4497,7 +4497,7 @@
         <v>61</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create Budget Delay Reduced
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Pictures\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegPack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="137">
   <si>
     <t>Description</t>
   </si>
@@ -433,6 +433,15 @@
   </si>
   <si>
     <t>CreateCompanyVendor</t>
+  </si>
+  <si>
+    <t>CreateClient</t>
+  </si>
+  <si>
+    <t>ClientCreation</t>
+  </si>
+  <si>
+    <t>Create Global Client,Brand,Product</t>
   </si>
 </sst>
 </file>
@@ -860,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,44 +920,32 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -968,20 +965,20 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
+      <c r="A4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
@@ -998,13 +995,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -1055,16 +1052,12 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1143,13 +1136,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
@@ -1171,17 +1164,17 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
+      <c r="A11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
@@ -1200,12 +1193,16 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12" s="3" t="s">
+      <c r="A12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1225,16 +1222,16 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="A13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1254,16 +1251,16 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="A14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1284,13 +1281,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
@@ -1313,13 +1310,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -1342,13 +1339,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -1371,13 +1368,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
@@ -1400,13 +1397,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>133</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1429,13 +1426,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
@@ -1458,13 +1455,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
@@ -1487,13 +1484,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
@@ -1516,13 +1513,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
@@ -1545,13 +1542,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1574,19 +1571,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>6</v>
@@ -1603,13 +1600,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1632,13 +1629,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
@@ -1661,13 +1658,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
@@ -1690,13 +1687,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1719,13 +1716,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>6</v>
@@ -1748,13 +1745,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -1777,13 +1774,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
@@ -1806,13 +1803,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
@@ -1835,13 +1832,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
@@ -1864,13 +1861,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
@@ -1893,13 +1890,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
@@ -1922,13 +1919,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>6</v>
@@ -1951,13 +1948,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>6</v>
@@ -1980,13 +1977,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -2009,13 +2006,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
@@ -2038,13 +2035,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>6</v>
@@ -2067,13 +2064,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
@@ -2096,13 +2093,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
@@ -2125,13 +2122,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -2154,13 +2151,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>6</v>
@@ -2183,13 +2180,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
@@ -2212,13 +2209,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
@@ -2241,13 +2238,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
@@ -2270,13 +2267,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>107</v>
+        <v>21</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -2299,13 +2296,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
@@ -2328,13 +2325,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>6</v>
@@ -2357,13 +2354,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
@@ -2386,13 +2383,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
@@ -2410,6 +2407,35 @@
         <v>6</v>
       </c>
       <c r="I53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating Test Case ID for JIRA(Sep Regression)
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Smoke Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -687,72 +687,6 @@
     <t>03. Create Employee Employee Vendor &amp; User</t>
   </si>
   <si>
-    <t>Create a Global Brand</t>
-  </si>
-  <si>
-    <t>Create a Global Product</t>
-  </si>
-  <si>
-    <t>Create a Company Client</t>
-  </si>
-  <si>
-    <t>Create a Company Brand</t>
-  </si>
-  <si>
-    <t>Create a Company Product</t>
-  </si>
-  <si>
-    <t>Amend a Global Client</t>
-  </si>
-  <si>
-    <t>Amend a Global Brand</t>
-  </si>
-  <si>
-    <t>Amend a Global Product</t>
-  </si>
-  <si>
-    <t>Amend a Company Client</t>
-  </si>
-  <si>
-    <t>Amend a Company Brand</t>
-  </si>
-  <si>
-    <t>Amend a Company Product</t>
-  </si>
-  <si>
-    <t>Block a Global Client</t>
-  </si>
-  <si>
-    <t>Block a Global Brand</t>
-  </si>
-  <si>
-    <t>Block a Company Product</t>
-  </si>
-  <si>
-    <t>Block a Company Brand</t>
-  </si>
-  <si>
-    <t>Block a Company Client</t>
-  </si>
-  <si>
-    <t>Block a Global Product</t>
-  </si>
-  <si>
-    <t>Create a Company Vendor</t>
-  </si>
-  <si>
-    <t>Amend a Global Vendor</t>
-  </si>
-  <si>
-    <t>Amend a Company Vendor</t>
-  </si>
-  <si>
-    <t>Block a Company Vendor</t>
-  </si>
-  <si>
-    <t>Block a Global Vendor</t>
-  </si>
-  <si>
     <t>01. Create a Payment Selection</t>
   </si>
   <si>
@@ -931,6 +865,72 @@
   </si>
   <si>
     <t>TM_Invoice</t>
+  </si>
+  <si>
+    <t>02. Create a Global Brand</t>
+  </si>
+  <si>
+    <t>03. Create a Global Product</t>
+  </si>
+  <si>
+    <t>04. Create a Company Client</t>
+  </si>
+  <si>
+    <t>05. Create a Company Brand</t>
+  </si>
+  <si>
+    <t>06. Create a Company Product</t>
+  </si>
+  <si>
+    <t>07. Amend a Global Client</t>
+  </si>
+  <si>
+    <t>08. Amend a Global Brand</t>
+  </si>
+  <si>
+    <t>09. Amend a Global Product</t>
+  </si>
+  <si>
+    <t>10. Amend a Company Client</t>
+  </si>
+  <si>
+    <t>11. Amend a Company Brand</t>
+  </si>
+  <si>
+    <t>12. Amend a Company Product</t>
+  </si>
+  <si>
+    <t>18. Block a Company Product</t>
+  </si>
+  <si>
+    <t>17. Block a Company Brand</t>
+  </si>
+  <si>
+    <t>16. Block a Company Client</t>
+  </si>
+  <si>
+    <t>15. Block a Global Product</t>
+  </si>
+  <si>
+    <t>14. Block a Global Brand</t>
+  </si>
+  <si>
+    <t>13. Block a Global Client</t>
+  </si>
+  <si>
+    <t>2. Create a Company Vendor</t>
+  </si>
+  <si>
+    <t>3. Amend a Global Vendor</t>
+  </si>
+  <si>
+    <t>4. Amend a Company Vendor</t>
+  </si>
+  <si>
+    <t>6. Block a Company Vendor</t>
+  </si>
+  <si>
+    <t>5. Block a Global Vendor</t>
   </si>
 </sst>
 </file>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,7 +1789,7 @@
         <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>89</v>
@@ -1807,7 +1807,7 @@
         <v>116</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>91</v>
@@ -2190,13 +2190,13 @@
         <v>161</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
@@ -2898,13 +2898,13 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>123</v>
@@ -3065,10 +3065,10 @@
         <v>179</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>128</v>
@@ -3147,7 +3147,7 @@
         <v>180</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>134</v>
@@ -3229,10 +3229,10 @@
         <v>181</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>128</v>
@@ -3311,7 +3311,7 @@
         <v>182</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>134</v>
@@ -3387,10 +3387,10 @@
         <v>184</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>128</v>
@@ -3946,16 +3946,16 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>6</v>
@@ -3987,16 +3987,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>6</v>
@@ -4028,16 +4028,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>6</v>
@@ -4069,16 +4069,16 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>6</v>
@@ -4110,12 +4110,12 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="2" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>6</v>
@@ -4273,10 +4273,10 @@
         <v>209</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>125</v>
@@ -4361,7 +4361,7 @@
         <v>16</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>6</v>
@@ -4402,7 +4402,7 @@
         <v>20</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>6</v>
@@ -4437,7 +4437,7 @@
         <v>213</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>6</v>
@@ -4472,7 +4472,7 @@
         <v>214</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>6</v>
@@ -4507,7 +4507,7 @@
         <v>215</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>6</v>
@@ -4548,7 +4548,7 @@
         <v>18</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>6</v>
@@ -4579,8 +4579,8 @@
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>217</v>
+      <c r="A71" t="s">
+        <v>277</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>99</v>
@@ -4620,8 +4620,8 @@
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>218</v>
+      <c r="A72" t="s">
+        <v>278</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>119</v>
@@ -4655,8 +4655,8 @@
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>219</v>
+      <c r="A73" t="s">
+        <v>279</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>119</v>
@@ -4690,8 +4690,8 @@
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>220</v>
+      <c r="A74" t="s">
+        <v>280</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>119</v>
@@ -4725,8 +4725,8 @@
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>221</v>
+      <c r="A75" t="s">
+        <v>281</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>119</v>
@@ -4760,8 +4760,8 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>222</v>
+      <c r="A76" t="s">
+        <v>282</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>84</v>
@@ -4801,8 +4801,8 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>223</v>
+      <c r="A77" t="s">
+        <v>283</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>119</v>
@@ -4836,8 +4836,8 @@
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>224</v>
+      <c r="A78" t="s">
+        <v>284</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>119</v>
@@ -4871,8 +4871,8 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>225</v>
+      <c r="A79" t="s">
+        <v>285</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>97</v>
@@ -4912,8 +4912,8 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>226</v>
+      <c r="A80" t="s">
+        <v>286</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>96</v>
@@ -4953,8 +4953,8 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>227</v>
+      <c r="A81" t="s">
+        <v>287</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>119</v>
@@ -4988,8 +4988,8 @@
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>230</v>
+      <c r="A82" t="s">
+        <v>288</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>79</v>
@@ -5029,8 +5029,8 @@
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>231</v>
+      <c r="A83" t="s">
+        <v>289</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>75</v>
@@ -5070,8 +5070,8 @@
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>232</v>
+      <c r="A84" t="s">
+        <v>290</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>119</v>
@@ -5105,8 +5105,8 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>233</v>
+      <c r="A85" t="s">
+        <v>291</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>119</v>
@@ -5140,8 +5140,8 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>229</v>
+      <c r="A86" t="s">
+        <v>292</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>119</v>
@@ -5175,8 +5175,8 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>228</v>
+      <c r="A87" t="s">
+        <v>293</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>70</v>
@@ -5216,8 +5216,8 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>234</v>
+      <c r="A88" t="s">
+        <v>294</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>6</v>
@@ -5248,8 +5248,8 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>235</v>
+      <c r="A89" t="s">
+        <v>295</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>6</v>
@@ -5280,8 +5280,8 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>236</v>
+      <c r="A90" t="s">
+        <v>296</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>6</v>
@@ -5312,8 +5312,8 @@
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>237</v>
+      <c r="A91" t="s">
+        <v>297</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>6</v>
@@ -5344,8 +5344,8 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>238</v>
+      <c r="A92" t="s">
+        <v>298</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>6</v>
@@ -5377,7 +5377,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>143</v>
@@ -5418,7 +5418,7 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>147</v>
@@ -5459,7 +5459,7 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>145</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>146</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>148</v>
@@ -5582,13 +5582,13 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>144</v>
@@ -5623,16 +5623,16 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>6</v>
@@ -5664,7 +5664,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>6</v>
@@ -5699,10 +5699,10 @@
         <v>127</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>127</v>
@@ -5737,16 +5737,16 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>6</v>
@@ -5778,16 +5778,16 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>6</v>
@@ -5819,16 +5819,16 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>6</v>
@@ -5860,16 +5860,16 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>6</v>
@@ -5901,16 +5901,16 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>6</v>
@@ -5942,16 +5942,16 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>285</v>
+        <v>263</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Updated Function Name in Runmanager for Fixed Asset Depriciation
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Smoke Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuite_BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:A92"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4235,13 +4235,13 @@
         <v>45</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>125</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Updated Change user and Employee
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuite_BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestAutomation1\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="307">
   <si>
     <t>Description</t>
   </si>
@@ -949,6 +949,12 @@
   </si>
   <si>
     <t>validatePaymentRemittanceMPL</t>
+  </si>
+  <si>
+    <t>changeEmployee</t>
+  </si>
+  <si>
+    <t>changeUser</t>
   </si>
 </sst>
 </file>
@@ -1706,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4317,7 +4323,7 @@
         <v>232</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>6</v>
@@ -4389,11 +4395,17 @@
       <c r="A67" s="2" t="s">
         <v>213</v>
       </c>
+      <c r="B67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>305</v>
+      </c>
       <c r="D67" s="2" t="s">
         <v>232</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>6</v>
@@ -4458,6 +4470,12 @@
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>215</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>306</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Updating Account Payable scripts
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -20,7 +20,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GlobalTestCase!$A$1:$O$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GlobalTestCase!$A$1:$O$113</definedName>
     <definedName name="IterationOptions">[1]Sheet1!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="328">
   <si>
     <t>Description</t>
   </si>
@@ -1110,332 +1110,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="88">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF321547"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF321547"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF321547"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF321547"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF321547"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2171,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O111"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,98 +2700,44 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>304</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>305</v>
+        <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>306</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>305</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>304</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>9</v>
+        <v>305</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>6</v>
@@ -3148,98 +2769,44 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>19</v>
+        <v>306</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>305</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>6</v>
@@ -3271,95 +2838,41 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>233</v>
+        <v>169</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>234</v>
+        <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>235</v>
+        <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>123</v>
@@ -3394,16 +2907,16 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>136</v>
+        <v>171</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>6</v>
@@ -3435,18 +2948,17 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="F31" s="2" t="s">
         <v>6</v>
       </c>
@@ -3477,16 +2989,16 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>133</v>
+        <v>19</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -3518,16 +3030,16 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>272</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>274</v>
+        <v>44</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>6</v>
@@ -3559,16 +3071,16 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>6</v>
@@ -3600,16 +3112,16 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>180</v>
+        <v>233</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>6</v>
@@ -3641,13 +3153,13 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>128</v>
@@ -3682,17 +3194,18 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>269</v>
+        <v>178</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D37" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>128</v>
       </c>
+      <c r="E37" s="6"/>
       <c r="F37" s="2" t="s">
         <v>6</v>
       </c>
@@ -3723,13 +3236,13 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>128</v>
@@ -3764,13 +3277,13 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>134</v>
+        <v>274</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>128</v>
@@ -3805,7 +3318,13 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>183</v>
+        <v>138</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>128</v>
@@ -3840,13 +3359,13 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>273</v>
+        <v>134</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>128</v>
@@ -3881,7 +3400,13 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>185</v>
+        <v>137</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>128</v>
@@ -3916,7 +3441,13 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>128</v>
@@ -3951,16 +3482,16 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>6</v>
@@ -3992,16 +3523,16 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>49</v>
+        <v>275</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>6</v>
@@ -4033,16 +3564,10 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>6</v>
@@ -4074,16 +3599,16 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>192</v>
+        <v>271</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>193</v>
+        <v>273</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>6</v>
@@ -4115,16 +3640,10 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>6</v>
@@ -4156,16 +3675,10 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>107</v>
+        <v>186</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>6</v>
@@ -4197,16 +3710,16 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>198</v>
+        <v>51</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>6</v>
@@ -4237,17 +3750,17 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>109</v>
+      <c r="A51" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>6</v>
@@ -4278,17 +3791,17 @@
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>200</v>
+      <c r="A52" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>107</v>
+        <v>190</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>6</v>
@@ -4320,180 +3833,180 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>113</v>
+        <v>192</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="F55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>6</v>
@@ -4525,299 +4038,299 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="F64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O64" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="2" t="s">
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O62" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O64" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>6</v>
@@ -4849,16 +4362,16 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>6</v>
@@ -4890,19 +4403,19 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>299</v>
+        <v>34</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>6</v>
@@ -4931,10 +4444,16 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>6</v>
@@ -4966,16 +4485,16 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>55</v>
+        <v>267</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>300</v>
+        <v>267</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>6</v>
@@ -5007,262 +4526,256 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O70" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O71" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O72" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O73" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O74" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O75" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O70" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>276</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O71" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>277</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O72" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>278</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>279</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>280</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>281</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>6</v>
@@ -5294,13 +4807,13 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>119</v>
@@ -5335,13 +4848,13 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>119</v>
@@ -5376,13 +4889,13 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>119</v>
@@ -5417,13 +4930,13 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>119</v>
@@ -5458,13 +4971,13 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>309</v>
+        <v>141</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>119</v>
@@ -5499,13 +5012,13 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>119</v>
@@ -5540,13 +5053,13 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>119</v>
@@ -5581,13 +5094,13 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>119</v>
@@ -5622,13 +5135,13 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>119</v>
@@ -5663,13 +5176,13 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>119</v>
@@ -5704,13 +5217,13 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>70</v>
+        <v>309</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>73</v>
+        <v>310</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>119</v>
@@ -5745,16 +5258,16 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>6</v>
@@ -5786,16 +5299,16 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>311</v>
+        <v>75</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>311</v>
+        <v>76</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>6</v>
@@ -5827,16 +5340,16 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>312</v>
+        <v>77</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>313</v>
+        <v>78</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>6</v>
@@ -5868,16 +5381,16 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>6</v>
@@ -5909,303 +5422,303 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>291</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O92" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>292</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O93" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>293</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O94" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>294</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O95" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>295</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N96" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O96" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>296</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O97" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>297</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O92" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="F98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O98" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O93" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O94" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O95" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O96" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O97" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O98" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>228</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>6</v>
@@ -6237,16 +5750,16 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>314</v>
+        <v>147</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>314</v>
+        <v>147</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>315</v>
+        <v>144</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>6</v>
@@ -6278,16 +5791,16 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>127</v>
+        <v>227</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>246</v>
+        <v>145</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>246</v>
+        <v>145</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>6</v>
@@ -6318,17 +5831,17 @@
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>259</v>
+      <c r="A102" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>248</v>
+        <v>146</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>249</v>
+        <v>146</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>250</v>
+        <v>144</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>6</v>
@@ -6359,17 +5872,17 @@
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>260</v>
+      <c r="A103" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>251</v>
+        <v>148</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>252</v>
+        <v>148</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>250</v>
+        <v>144</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>6</v>
@@ -6400,17 +5913,17 @@
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>261</v>
+      <c r="A104" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>250</v>
+        <v>144</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>6</v>
@@ -6442,16 +5955,16 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>6</v>
@@ -6482,17 +5995,17 @@
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>262</v>
+      <c r="A106" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>258</v>
+        <v>314</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>250</v>
+        <v>315</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>6</v>
@@ -6523,17 +6036,17 @@
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>263</v>
+      <c r="A107" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>258</v>
+        <v>246</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>250</v>
+        <v>127</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>6</v>
@@ -6565,13 +6078,13 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>322</v>
+        <v>259</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>316</v>
+        <v>248</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>317</v>
+        <v>249</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>250</v>
@@ -6606,13 +6119,13 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>323</v>
+        <v>260</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>298</v>
+        <v>251</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>250</v>
@@ -6647,188 +6160,434 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>324</v>
+        <v>261</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>318</v>
+        <v>253</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>319</v>
+        <v>254</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="F110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O110" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>325</v>
+        <v>264</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>320</v>
+        <v>255</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>321</v>
+        <v>256</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="F111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O111" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>262</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O112" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>263</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O113" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>322</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N114" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O114" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>323</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N115" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O115" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>324</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>325</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O107"/>
-  <conditionalFormatting sqref="A102">
+  <autoFilter ref="A1:O113"/>
+  <conditionalFormatting sqref="A108">
     <cfRule type="expression" dxfId="47" priority="41">
-      <formula>$R102="Passed"</formula>
+      <formula>$R108="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="46" priority="42">
-      <formula>$R102="Not Ready"</formula>
+      <formula>$R108="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="45" priority="43">
-      <formula>$R102="Retest"</formula>
+      <formula>$R108="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="44" priority="44">
-      <formula>$R102="Query"</formula>
+      <formula>$R108="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="43" priority="45">
-      <formula>$R102="Blocked"</formula>
+      <formula>$R108="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="42" priority="46">
-      <formula>$R102="In Progress"</formula>
+      <formula>$R108="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="41" priority="47">
-      <formula>$R102="N/A"</formula>
+      <formula>$R108="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="48">
-      <formula>$R102="Failed"</formula>
+      <formula>$R108="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103">
+  <conditionalFormatting sqref="A109">
     <cfRule type="expression" dxfId="39" priority="33">
-      <formula>$R103="Passed"</formula>
+      <formula>$R109="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="38" priority="34">
-      <formula>$R103="Not Ready"</formula>
+      <formula>$R109="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="37" priority="35">
-      <formula>$R103="Retest"</formula>
+      <formula>$R109="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="36">
-      <formula>$R103="Query"</formula>
+      <formula>$R109="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="35" priority="37">
-      <formula>$R103="Blocked"</formula>
+      <formula>$R109="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="38">
-      <formula>$R103="In Progress"</formula>
+      <formula>$R109="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="39">
-      <formula>$R103="N/A"</formula>
+      <formula>$R109="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="32" priority="40">
-      <formula>$R103="Failed"</formula>
+      <formula>$R109="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A104">
+  <conditionalFormatting sqref="A110">
     <cfRule type="expression" dxfId="31" priority="25">
-      <formula>$R104="Passed"</formula>
+      <formula>$R110="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="30" priority="26">
-      <formula>$R104="Not Ready"</formula>
+      <formula>$R110="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="29" priority="27">
-      <formula>$R104="Retest"</formula>
+      <formula>$R110="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="28">
-      <formula>$R104="Query"</formula>
+      <formula>$R110="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="27" priority="29">
-      <formula>$R104="Blocked"</formula>
+      <formula>$R110="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="30">
-      <formula>$R104="In Progress"</formula>
+      <formula>$R110="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="31">
-      <formula>$R104="N/A"</formula>
+      <formula>$R110="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="24" priority="32">
-      <formula>$R104="Failed"</formula>
+      <formula>$R110="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A106">
+  <conditionalFormatting sqref="A112">
     <cfRule type="expression" dxfId="23" priority="17">
-      <formula>$R106="Passed"</formula>
+      <formula>$R112="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="18">
-      <formula>$R106="Not Ready"</formula>
+      <formula>$R112="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="19">
-      <formula>$R106="Retest"</formula>
+      <formula>$R112="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="20" priority="20">
-      <formula>$R106="Query"</formula>
+      <formula>$R112="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="21">
-      <formula>$R106="Blocked"</formula>
+      <formula>$R112="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="22">
-      <formula>$R106="In Progress"</formula>
+      <formula>$R112="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="17" priority="23">
-      <formula>$R106="N/A"</formula>
+      <formula>$R112="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="24">
-      <formula>$R106="Failed"</formula>
+      <formula>$R112="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A107">
+  <conditionalFormatting sqref="A113">
     <cfRule type="expression" dxfId="15" priority="9">
-      <formula>$R107="Passed"</formula>
+      <formula>$R113="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="14" priority="10">
-      <formula>$R107="Not Ready"</formula>
+      <formula>$R113="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="11">
-      <formula>$R107="Retest"</formula>
+      <formula>$R113="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="12">
-      <formula>$R107="Query"</formula>
+      <formula>$R113="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="13">
-      <formula>$R107="Blocked"</formula>
+      <formula>$R113="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="14">
-      <formula>$R107="In Progress"</formula>
+      <formula>$R113="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="15">
-      <formula>$R107="N/A"</formula>
+      <formula>$R113="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="16">
-      <formula>$R107="Failed"</formula>
+      <formula>$R113="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A105">
+  <conditionalFormatting sqref="A111">
     <cfRule type="expression" dxfId="7" priority="1">
-      <formula>$R105="Passed"</formula>
+      <formula>$R111="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$R105="Not Ready"</formula>
+      <formula>$R111="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="3">
-      <formula>$R105="Retest"</formula>
+      <formula>$R111="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="4">
-      <formula>$R105="Query"</formula>
+      <formula>$R111="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="5">
-      <formula>$R105="Blocked"</formula>
+      <formula>$R111="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>$R105="In Progress"</formula>
+      <formula>$R111="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="7">
-      <formula>$R105="N/A"</formula>
+      <formula>$R111="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>$R105="Failed"</formula>
+      <formula>$R111="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating Job Creation scripts
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="329">
   <si>
     <t>Description</t>
   </si>
@@ -1018,6 +1018,9 @@
   </si>
   <si>
     <t>UAE_Regression</t>
+  </si>
+  <si>
+    <t>Job_Creation</t>
   </si>
 </sst>
 </file>
@@ -1848,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,7 +2012,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>328</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
Updating NameMapping for Job Crediting
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -20,7 +20,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GlobalTestCase!$A$1:$O$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GlobalTestCase!$A$1:$O$115</definedName>
     <definedName name="IterationOptions">[1]Sheet1!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="341">
   <si>
     <t>Description</t>
   </si>
@@ -1033,6 +1033,30 @@
   </si>
   <si>
     <t>Create_Blanket_Invoice</t>
+  </si>
+  <si>
+    <t>Create_Job_Creaditing</t>
+  </si>
+  <si>
+    <t>Job_Crediting</t>
+  </si>
+  <si>
+    <t>Import Budget Model</t>
+  </si>
+  <si>
+    <t>Import_Budget_Model</t>
+  </si>
+  <si>
+    <t>Import_Budget_Template</t>
+  </si>
+  <si>
+    <t>Update_Perodic_Balance</t>
+  </si>
+  <si>
+    <t>Updating_Perodic_Balance</t>
+  </si>
+  <si>
+    <t>Update Periodic Balance</t>
   </si>
 </sst>
 </file>
@@ -1868,10 +1892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O117"/>
+  <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3670,6 +3694,12 @@
       <c r="A48" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="B48" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>333</v>
+      </c>
       <c r="D48" s="2" t="s">
         <v>128</v>
       </c>
@@ -3949,54 +3979,27 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>196</v>
+        <v>335</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>106</v>
+        <v>336</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>107</v>
+        <v>337</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>198</v>
+        <v>106</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>127</v>
@@ -4030,14 +4033,14 @@
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>109</v>
+      <c r="A57" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>127</v>
@@ -4071,14 +4074,14 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>107</v>
+      <c r="A58" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>127</v>
@@ -4112,14 +4115,14 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>113</v>
+      <c r="A59" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>201</v>
+        <v>107</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>127</v>
@@ -4153,14 +4156,14 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>109</v>
+      <c r="A60" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>127</v>
@@ -4195,16 +4198,16 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>238</v>
+        <v>111</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>242</v>
+        <v>127</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>6</v>
@@ -4236,13 +4239,13 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>237</v>
+        <v>217</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>242</v>
@@ -4277,13 +4280,13 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>247</v>
+        <v>218</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>242</v>
@@ -4318,13 +4321,13 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>242</v>
@@ -4359,10 +4362,14 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
+        <v>220</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>241</v>
+      </c>
       <c r="D65" s="2" t="s">
         <v>242</v>
       </c>
@@ -4395,17 +4402,13 @@
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="A66" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
       <c r="D66" s="2" t="s">
-        <v>125</v>
+        <v>242</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>6</v>
@@ -4437,13 +4440,13 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>125</v>
@@ -4478,13 +4481,13 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>125</v>
@@ -4519,13 +4522,13 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>125</v>
@@ -4560,13 +4563,13 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>35</v>
+        <v>267</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>307</v>
+        <v>267</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>125</v>
@@ -4601,16 +4604,16 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>6</v>
@@ -4642,13 +4645,13 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>232</v>
@@ -4683,19 +4686,19 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>299</v>
+        <v>20</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>232</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>6</v>
@@ -4724,13 +4727,19 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>299</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>232</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>6</v>
@@ -4759,13 +4768,7 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>300</v>
+        <v>214</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>232</v>
@@ -4800,13 +4803,13 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>18</v>
+        <v>300</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>232</v>
@@ -4840,17 +4843,17 @@
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>276</v>
+      <c r="A77" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>119</v>
+        <v>232</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>6</v>
@@ -4882,13 +4885,13 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>119</v>
@@ -4923,13 +4926,13 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>119</v>
@@ -4964,13 +4967,13 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>119</v>
@@ -5005,13 +5008,13 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>308</v>
+        <v>93</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>119</v>
@@ -5046,13 +5049,13 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>84</v>
+        <v>308</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>119</v>
@@ -5087,13 +5090,13 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>119</v>
@@ -5128,13 +5131,13 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>119</v>
@@ -5169,13 +5172,13 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>119</v>
@@ -5210,13 +5213,13 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>119</v>
@@ -5251,13 +5254,13 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>309</v>
+        <v>96</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>310</v>
+        <v>96</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>119</v>
@@ -5292,13 +5295,13 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>79</v>
+        <v>309</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>80</v>
+        <v>310</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>119</v>
@@ -5333,13 +5336,13 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>119</v>
@@ -5374,13 +5377,13 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>119</v>
@@ -5415,13 +5418,13 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>119</v>
@@ -5456,13 +5459,13 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>119</v>
@@ -5497,13 +5500,13 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>119</v>
@@ -5538,16 +5541,16 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>6</v>
@@ -5579,13 +5582,13 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>311</v>
+        <v>102</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>311</v>
+        <v>103</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>301</v>
@@ -5620,13 +5623,13 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>301</v>
@@ -5661,13 +5664,13 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>83</v>
+        <v>312</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>83</v>
+        <v>313</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>301</v>
@@ -5702,13 +5705,13 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>301</v>
@@ -5742,17 +5745,17 @@
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>225</v>
+      <c r="A99" t="s">
+        <v>297</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>144</v>
+        <v>301</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>6</v>
@@ -5783,55 +5786,28 @@
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>226</v>
+      <c r="A100" t="s">
+        <v>340</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>147</v>
+        <v>338</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>147</v>
+        <v>339</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O100" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>144</v>
@@ -5866,13 +5842,13 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>144</v>
@@ -5907,13 +5883,13 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>144</v>
@@ -5948,13 +5924,13 @@
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>266</v>
+        <v>146</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>266</v>
+        <v>146</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>144</v>
@@ -5988,17 +5964,17 @@
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>228</v>
+      <c r="A105" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>245</v>
+        <v>148</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>245</v>
+        <v>148</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>245</v>
+        <v>144</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>6</v>
@@ -6030,139 +6006,139 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O106" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>228</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O107" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D108" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O106" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+      <c r="F108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N108" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O108" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D109" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O107" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>259</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O108" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>260</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>6</v>
@@ -6194,13 +6170,13 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>250</v>
@@ -6235,13 +6211,13 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>250</v>
@@ -6276,13 +6252,13 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>258</v>
+        <v>253</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>250</v>
@@ -6317,13 +6293,13 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>258</v>
+        <v>255</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>250</v>
@@ -6358,13 +6334,13 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>322</v>
+        <v>262</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>317</v>
+        <v>257</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>258</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>250</v>
@@ -6399,13 +6375,13 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>323</v>
+        <v>263</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>238</v>
+        <v>265</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>258</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>250</v>
@@ -6440,188 +6416,270 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="F116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O116" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>321</v>
+        <v>238</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="F117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O117" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>324</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>325</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O113"/>
-  <conditionalFormatting sqref="A108">
+  <autoFilter ref="A1:O115"/>
+  <conditionalFormatting sqref="A110">
     <cfRule type="expression" dxfId="47" priority="41">
-      <formula>$R108="Passed"</formula>
+      <formula>$R110="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="46" priority="42">
-      <formula>$R108="Not Ready"</formula>
+      <formula>$R110="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="45" priority="43">
-      <formula>$R108="Retest"</formula>
+      <formula>$R110="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="44" priority="44">
-      <formula>$R108="Query"</formula>
+      <formula>$R110="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="43" priority="45">
-      <formula>$R108="Blocked"</formula>
+      <formula>$R110="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="42" priority="46">
-      <formula>$R108="In Progress"</formula>
+      <formula>$R110="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="41" priority="47">
-      <formula>$R108="N/A"</formula>
+      <formula>$R110="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="48">
-      <formula>$R108="Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A109">
-    <cfRule type="expression" dxfId="39" priority="33">
-      <formula>$R109="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
-      <formula>$R109="Not Ready"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
-      <formula>$R109="Retest"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
-      <formula>$R109="Query"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="37">
-      <formula>$R109="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
-      <formula>$R109="In Progress"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
-      <formula>$R109="N/A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="40">
-      <formula>$R109="Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A110">
-    <cfRule type="expression" dxfId="31" priority="25">
-      <formula>$R110="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
-      <formula>$R110="Not Ready"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
-      <formula>$R110="Retest"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
-      <formula>$R110="Query"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>$R110="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
-      <formula>$R110="In Progress"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>$R110="N/A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
       <formula>$R110="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A111">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>$R111="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>$R111="Not Ready"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>$R111="Retest"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>$R111="Query"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>$R111="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>$R111="In Progress"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>$R111="N/A"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>$R111="Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A112">
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="31" priority="25">
       <formula>$R112="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="30" priority="26">
       <formula>$R112="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="29" priority="27">
       <formula>$R112="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="28" priority="28">
       <formula>$R112="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>$R112="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="26" priority="30">
       <formula>$R112="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="25" priority="31">
       <formula>$R112="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
+    <cfRule type="expression" dxfId="24" priority="32">
       <formula>$R112="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A114">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>$R114="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>$R114="Not Ready"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>$R114="Retest"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>$R114="Query"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>$R114="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>$R114="In Progress"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>$R114="N/A"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>$R114="Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A115">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>$R115="Passed"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>$R115="Not Ready"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>$R115="Retest"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>$R115="Query"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>$R115="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>$R115="In Progress"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>$R115="N/A"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>$R115="Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A113">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$R113="Passed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$R113="Not Ready"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$R113="Retest"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$R113="Query"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$R113="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$R113="In Progress"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$R113="N/A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>$R113="Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A111">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>$R111="Passed"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$R111="Not Ready"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>$R111="Retest"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>$R111="Query"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>$R111="Blocked"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>$R111="In Progress"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
-      <formula>$R111="N/A"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
-      <formula>$R111="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Draft and CreditNote MPL Scripts
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\OneDrive - Cognizant\Documents\WPP Global TestScripts\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="345">
   <si>
     <t>Description</t>
   </si>
@@ -1057,6 +1057,18 @@
   </si>
   <si>
     <t>Update Periodic Balance</t>
+  </si>
+  <si>
+    <t>DraftCreditMemo</t>
+  </si>
+  <si>
+    <t>DraftCreditMemo_MPL</t>
+  </si>
+  <si>
+    <t>CreditMemo</t>
+  </si>
+  <si>
+    <t>CreditMemo_MPL</t>
   </si>
 </sst>
 </file>
@@ -1892,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6339,7 +6351,7 @@
       <c r="B114" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="C114" s="2" t="s">
         <v>258</v>
       </c>
       <c r="D114" s="2" t="s">
@@ -6380,8 +6392,8 @@
       <c r="B115" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C115" s="6" t="s">
-        <v>258</v>
+      <c r="C115" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>250</v>
@@ -6509,6 +6521,33 @@
       <c r="D118" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="F118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O118" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -6522,6 +6561,115 @@
       </c>
       <c r="D119" s="2" t="s">
         <v>250</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O119" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O120" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O121" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Bank_Reconciliation and Inprogress MPL's
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -20,7 +20,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GlobalTestCase!$A$1:$O$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GlobalTestCase!$A$1:$M$121</definedName>
     <definedName name="IterationOptions">[1]Sheet1!$A$2:$A$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="360">
   <si>
     <t>Description</t>
   </si>
@@ -1059,49 +1059,61 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Validate Job Quotation MPL</t>
-  </si>
-  <si>
-    <t>Validate Job Order Confirmation MPL</t>
-  </si>
-  <si>
-    <t>Validate Job Budget - Estimate MPL</t>
-  </si>
-  <si>
-    <t>Validate General Journal MPL</t>
-  </si>
-  <si>
-    <t>Validate Draft Invoice MPL</t>
-  </si>
-  <si>
-    <t>Validate Invoice MPL</t>
-  </si>
-  <si>
-    <t>Validate Payment Order MPL</t>
-  </si>
-  <si>
-    <t>Validate Payment Selection MPL</t>
-  </si>
-  <si>
-    <t>Validate Time Sheet MPL</t>
-  </si>
-  <si>
-    <t>Validate Expense Sheet MPL</t>
-  </si>
-  <si>
-    <t>Validate DraftCreditMemo MPL</t>
-  </si>
-  <si>
-    <t>Validate CreditMemo MPL</t>
-  </si>
-  <si>
-    <t>Validate PurchaseOrder MPL</t>
-  </si>
-  <si>
     <t>PurchaseOrder_MPL</t>
   </si>
   <si>
     <t>PurchaseOrderMPL</t>
+  </si>
+  <si>
+    <t>Purchase Order</t>
+  </si>
+  <si>
+    <t>Draft Invoice</t>
+  </si>
+  <si>
+    <t>Draft Credit Note</t>
+  </si>
+  <si>
+    <t>Bank Reconciliation in Progress</t>
+  </si>
+  <si>
+    <t>Bank Reconciliation</t>
+  </si>
+  <si>
+    <t>Time Sheet</t>
+  </si>
+  <si>
+    <t>Job Quotation</t>
+  </si>
+  <si>
+    <t>Payment Order</t>
+  </si>
+  <si>
+    <t>Job Order Confirmation</t>
+  </si>
+  <si>
+    <t>Payment Selection</t>
+  </si>
+  <si>
+    <t>Credit Note</t>
+  </si>
+  <si>
+    <t>Job Budget - Estimate</t>
+  </si>
+  <si>
+    <t>General Journal</t>
+  </si>
+  <si>
+    <t>Expense Sheet</t>
+  </si>
+  <si>
+    <t>BankingReconciliation_MPL</t>
+  </si>
+  <si>
+    <t>Banking_Reconciliation_InProgress</t>
+  </si>
+  <si>
+    <t>BankingReconciliation_InProgress_MPL</t>
   </si>
 </sst>
 </file>
@@ -1931,32 +1943,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O122"/>
+  <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82" style="2" customWidth="1"/>
+    <col min="1" max="1" width="52" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="25.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
@@ -1970,40 +1981,34 @@
         <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>86</v>
+        <v>316</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>316</v>
+        <v>230</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>149</v>
       </c>
@@ -2022,13 +2027,13 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -2037,14 +2042,8 @@
       <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>150</v>
       </c>
@@ -2063,13 +2062,13 @@
       <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -2078,14 +2077,8 @@
       <c r="M3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>152</v>
       </c>
@@ -2104,13 +2097,13 @@
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -2119,14 +2112,8 @@
       <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>153</v>
       </c>
@@ -2145,13 +2132,13 @@
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -2160,14 +2147,8 @@
       <c r="M5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>154</v>
       </c>
@@ -2186,13 +2167,13 @@
       <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -2201,14 +2182,8 @@
       <c r="M6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>155</v>
       </c>
@@ -2227,13 +2202,13 @@
       <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -2242,14 +2217,8 @@
       <c r="M7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>335</v>
       </c>
@@ -2268,13 +2237,13 @@
       <c r="F8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -2283,14 +2252,8 @@
       <c r="M8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>159</v>
       </c>
@@ -2309,13 +2272,13 @@
       <c r="F9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -2324,14 +2287,8 @@
       <c r="M9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>157</v>
       </c>
@@ -2350,13 +2307,13 @@
       <c r="F10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L10" s="2" t="s">
@@ -2365,14 +2322,8 @@
       <c r="M10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>161</v>
       </c>
@@ -2391,13 +2342,13 @@
       <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -2406,14 +2357,8 @@
       <c r="M11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>158</v>
       </c>
@@ -2432,13 +2377,13 @@
       <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L12" s="2" t="s">
@@ -2447,14 +2392,8 @@
       <c r="M12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>160</v>
       </c>
@@ -2473,13 +2412,13 @@
       <c r="F13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L13" s="2" t="s">
@@ -2488,14 +2427,8 @@
       <c r="M13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>159</v>
       </c>
@@ -2514,13 +2447,13 @@
       <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L14" s="2" t="s">
@@ -2529,14 +2462,8 @@
       <c r="M14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>175</v>
       </c>
@@ -2555,13 +2482,13 @@
       <c r="F15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L15" s="2" t="s">
@@ -2570,14 +2497,8 @@
       <c r="M15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>162</v>
       </c>
@@ -2596,13 +2517,13 @@
       <c r="F16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L16" s="2" t="s">
@@ -2611,14 +2532,8 @@
       <c r="M16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>165</v>
       </c>
@@ -2637,13 +2552,13 @@
       <c r="F17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L17" s="2" t="s">
@@ -2652,14 +2567,8 @@
       <c r="M17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>163</v>
       </c>
@@ -2678,13 +2587,13 @@
       <c r="F18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L18" s="2" t="s">
@@ -2693,14 +2602,8 @@
       <c r="M18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -2719,13 +2622,13 @@
       <c r="F19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L19" s="2" t="s">
@@ -2734,14 +2637,8 @@
       <c r="M19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>166</v>
       </c>
@@ -2760,13 +2657,13 @@
       <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L20" s="2" t="s">
@@ -2775,14 +2672,8 @@
       <c r="M20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>163</v>
       </c>
@@ -2798,8 +2689,11 @@
       <c r="E21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>164</v>
       </c>
@@ -2815,8 +2709,11 @@
       <c r="E22" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>167</v>
       </c>
@@ -2835,13 +2732,13 @@
       <c r="F23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L23" s="2" t="s">
@@ -2850,14 +2747,8 @@
       <c r="M23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>163</v>
       </c>
@@ -2873,8 +2764,11 @@
       <c r="E24" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>164</v>
       </c>
@@ -2890,8 +2784,11 @@
       <c r="E25" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>168</v>
       </c>
@@ -2910,13 +2807,13 @@
       <c r="F26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L26" s="2" t="s">
@@ -2925,14 +2822,8 @@
       <c r="M26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>163</v>
       </c>
@@ -2948,8 +2839,11 @@
       <c r="E27" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>164</v>
       </c>
@@ -2965,8 +2859,11 @@
       <c r="E28" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>169</v>
       </c>
@@ -2985,13 +2882,13 @@
       <c r="F29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L29" s="2" t="s">
@@ -3000,14 +2897,8 @@
       <c r="M29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>171</v>
       </c>
@@ -3026,13 +2917,13 @@
       <c r="F30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L30" s="2" t="s">
@@ -3041,14 +2932,8 @@
       <c r="M30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>170</v>
       </c>
@@ -3067,13 +2952,13 @@
       <c r="F31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L31" s="2" t="s">
@@ -3082,14 +2967,8 @@
       <c r="M31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>172</v>
       </c>
@@ -3108,13 +2987,13 @@
       <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L32" s="2" t="s">
@@ -3123,14 +3002,8 @@
       <c r="M32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -3149,13 +3022,13 @@
       <c r="F33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L33" s="2" t="s">
@@ -3164,14 +3037,8 @@
       <c r="M33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>173</v>
       </c>
@@ -3190,13 +3057,13 @@
       <c r="F34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L34" s="2" t="s">
@@ -3205,14 +3072,8 @@
       <c r="M34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>233</v>
       </c>
@@ -3231,13 +3092,13 @@
       <c r="F35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L35" s="2" t="s">
@@ -3246,14 +3107,8 @@
       <c r="M35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>136</v>
       </c>
@@ -3272,13 +3127,13 @@
       <c r="F36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L36" s="2" t="s">
@@ -3287,14 +3142,8 @@
       <c r="M36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>176</v>
       </c>
@@ -3313,14 +3162,14 @@
       <c r="F37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="G37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="6"/>
       <c r="I37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L37" s="2" t="s">
@@ -3329,14 +3178,8 @@
       <c r="M37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>140</v>
       </c>
@@ -3355,13 +3198,13 @@
       <c r="F38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L38" s="2" t="s">
@@ -3370,14 +3213,8 @@
       <c r="M38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>179</v>
       </c>
@@ -3396,13 +3233,13 @@
       <c r="F39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L39" s="2" t="s">
@@ -3411,14 +3248,8 @@
       <c r="M39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>138</v>
       </c>
@@ -3437,13 +3268,13 @@
       <c r="F40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L40" s="2" t="s">
@@ -3452,14 +3283,8 @@
       <c r="M40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>180</v>
       </c>
@@ -3478,13 +3303,13 @@
       <c r="F41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L41" s="2" t="s">
@@ -3493,14 +3318,8 @@
       <c r="M41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>137</v>
       </c>
@@ -3519,13 +3338,13 @@
       <c r="F42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L42" s="2" t="s">
@@ -3534,14 +3353,8 @@
       <c r="M42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>181</v>
       </c>
@@ -3560,13 +3373,13 @@
       <c r="F43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L43" s="2" t="s">
@@ -3575,14 +3388,8 @@
       <c r="M43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>139</v>
       </c>
@@ -3601,13 +3408,13 @@
       <c r="F44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="K44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L44" s="2" t="s">
@@ -3616,14 +3423,8 @@
       <c r="M44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O44" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>182</v>
       </c>
@@ -3642,13 +3443,13 @@
       <c r="F45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="K45" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L45" s="2" t="s">
@@ -3657,14 +3458,8 @@
       <c r="M45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>183</v>
       </c>
@@ -3680,16 +3475,16 @@
       <c r="E46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H46" s="7" t="s">
+      <c r="F46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J46" s="7" t="s">
+      <c r="K46" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L46" s="7" t="s">
@@ -3698,14 +3493,8 @@
       <c r="M46" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N46" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O46" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>184</v>
       </c>
@@ -3721,16 +3510,16 @@
       <c r="E47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="7" t="s">
+      <c r="F47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J47" s="7" t="s">
+      <c r="K47" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L47" s="7" t="s">
@@ -3739,14 +3528,8 @@
       <c r="M47" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N47" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O47" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>185</v>
       </c>
@@ -3762,16 +3545,16 @@
       <c r="E48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F48" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" s="7" t="s">
+      <c r="F48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J48" s="7" t="s">
+      <c r="K48" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L48" s="7" t="s">
@@ -3780,14 +3563,8 @@
       <c r="M48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N48" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O48" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>186</v>
       </c>
@@ -3803,16 +3580,16 @@
       <c r="E49" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" s="7" t="s">
+      <c r="F49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J49" s="7" t="s">
+      <c r="K49" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L49" s="7" t="s">
@@ -3821,14 +3598,8 @@
       <c r="M49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N49" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O49" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>187</v>
       </c>
@@ -3847,13 +3618,13 @@
       <c r="F50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="K50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L50" s="2" t="s">
@@ -3862,14 +3633,8 @@
       <c r="M50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N50" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>188</v>
       </c>
@@ -3888,13 +3653,13 @@
       <c r="F51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="K51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L51" s="2" t="s">
@@ -3903,14 +3668,8 @@
       <c r="M51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O51" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>194</v>
       </c>
@@ -3929,13 +3688,13 @@
       <c r="F52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="K52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L52" s="2" t="s">
@@ -3944,14 +3703,8 @@
       <c r="M52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O52" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>191</v>
       </c>
@@ -3970,13 +3723,13 @@
       <c r="F53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="K53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L53" s="2" t="s">
@@ -3985,14 +3738,8 @@
       <c r="M53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O53" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>195</v>
       </c>
@@ -4011,13 +3758,13 @@
       <c r="F54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="K54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L54" s="2" t="s">
@@ -4026,14 +3773,8 @@
       <c r="M54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>324</v>
       </c>
@@ -4049,8 +3790,11 @@
       <c r="E55" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>196</v>
       </c>
@@ -4069,13 +3813,13 @@
       <c r="F56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J56" s="2" t="s">
+      <c r="K56" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L56" s="2" t="s">
@@ -4084,14 +3828,8 @@
       <c r="M56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O56" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>197</v>
       </c>
@@ -4110,13 +3848,13 @@
       <c r="F57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="2" t="s">
+      <c r="K57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L57" s="2" t="s">
@@ -4125,14 +3863,8 @@
       <c r="M57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>202</v>
       </c>
@@ -4151,13 +3883,13 @@
       <c r="F58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J58" s="2" t="s">
+      <c r="K58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L58" s="2" t="s">
@@ -4166,14 +3898,8 @@
       <c r="M58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O58" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>203</v>
       </c>
@@ -4192,13 +3918,13 @@
       <c r="F59" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="K59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L59" s="2" t="s">
@@ -4207,14 +3933,8 @@
       <c r="M59" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>204</v>
       </c>
@@ -4233,13 +3953,13 @@
       <c r="F60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J60" s="2" t="s">
+      <c r="K60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L60" s="2" t="s">
@@ -4248,14 +3968,8 @@
       <c r="M60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>205</v>
       </c>
@@ -4274,13 +3988,13 @@
       <c r="F61" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J61" s="2" t="s">
+      <c r="K61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L61" s="2" t="s">
@@ -4289,14 +4003,8 @@
       <c r="M61" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O61" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>217</v>
       </c>
@@ -4313,15 +4021,15 @@
         <v>6</v>
       </c>
       <c r="F62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I62" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J62" s="2" t="s">
+      <c r="K62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L62" s="2" t="s">
@@ -4330,14 +4038,8 @@
       <c r="M62" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O62" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>218</v>
       </c>
@@ -4356,13 +4058,13 @@
       <c r="F63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J63" s="2" t="s">
+      <c r="K63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L63" s="2" t="s">
@@ -4371,14 +4073,8 @@
       <c r="M63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O63" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>219</v>
       </c>
@@ -4395,15 +4091,15 @@
         <v>6</v>
       </c>
       <c r="F64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="K64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L64" s="2" t="s">
@@ -4412,14 +4108,8 @@
       <c r="M64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O64" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>220</v>
       </c>
@@ -4436,15 +4126,15 @@
         <v>6</v>
       </c>
       <c r="F65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I65" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="K65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L65" s="2" t="s">
@@ -4453,14 +4143,8 @@
       <c r="M65" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O65" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>221</v>
       </c>
@@ -4479,13 +4163,13 @@
       <c r="F66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="K66" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L66" s="2" t="s">
@@ -4494,14 +4178,8 @@
       <c r="M66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N66" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O66" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>338</v>
       </c>
@@ -4515,16 +4193,16 @@
         <v>242</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>6</v>
+        <v>340</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>206</v>
       </c>
@@ -4543,13 +4221,13 @@
       <c r="F68" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="K68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L68" s="2" t="s">
@@ -4558,14 +4236,8 @@
       <c r="M68" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O68" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>207</v>
       </c>
@@ -4584,13 +4256,13 @@
       <c r="F69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="K69" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L69" s="2" t="s">
@@ -4599,14 +4271,8 @@
       <c r="M69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N69" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O69" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>208</v>
       </c>
@@ -4625,13 +4291,13 @@
       <c r="F70" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="K70" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L70" s="2" t="s">
@@ -4640,14 +4306,8 @@
       <c r="M70" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N70" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O70" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>209</v>
       </c>
@@ -4666,13 +4326,13 @@
       <c r="F71" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="K71" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L71" s="2" t="s">
@@ -4681,14 +4341,8 @@
       <c r="M71" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N71" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O71" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>210</v>
       </c>
@@ -4707,13 +4361,13 @@
       <c r="F72" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J72" s="2" t="s">
+      <c r="K72" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L72" s="2" t="s">
@@ -4722,14 +4376,8 @@
       <c r="M72" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N72" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O72" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>211</v>
       </c>
@@ -4748,13 +4396,13 @@
       <c r="F73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="K73" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L73" s="2" t="s">
@@ -4763,14 +4411,8 @@
       <c r="M73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>212</v>
       </c>
@@ -4789,13 +4431,13 @@
       <c r="F74" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L74" s="2" t="s">
@@ -4804,14 +4446,8 @@
       <c r="M74" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>213</v>
       </c>
@@ -4830,13 +4466,13 @@
       <c r="F75" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="K75" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L75" s="2" t="s">
@@ -4845,14 +4481,8 @@
       <c r="M75" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>214</v>
       </c>
@@ -4865,13 +4495,13 @@
       <c r="F76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="K76" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L76" s="2" t="s">
@@ -4880,14 +4510,8 @@
       <c r="M76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N76" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O76" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>215</v>
       </c>
@@ -4906,13 +4530,13 @@
       <c r="F77" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J77" s="2" t="s">
+      <c r="K77" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L77" s="2" t="s">
@@ -4921,14 +4545,8 @@
       <c r="M77" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N77" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O77" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>216</v>
       </c>
@@ -4947,13 +4565,13 @@
       <c r="F78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="K78" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L78" s="2" t="s">
@@ -4962,14 +4580,8 @@
       <c r="M78" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N78" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O78" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>270</v>
       </c>
@@ -4988,13 +4600,13 @@
       <c r="F79" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J79" s="2" t="s">
+      <c r="K79" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L79" s="2" t="s">
@@ -5003,14 +4615,8 @@
       <c r="M79" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O79" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>271</v>
       </c>
@@ -5029,13 +4635,13 @@
       <c r="F80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J80" s="2" t="s">
+      <c r="K80" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L80" s="2" t="s">
@@ -5044,14 +4650,8 @@
       <c r="M80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N80" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>272</v>
       </c>
@@ -5070,13 +4670,13 @@
       <c r="F81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="K81" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L81" s="2" t="s">
@@ -5085,14 +4685,8 @@
       <c r="M81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N81" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O81" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>273</v>
       </c>
@@ -5111,13 +4705,13 @@
       <c r="F82" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="K82" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L82" s="2" t="s">
@@ -5126,14 +4720,8 @@
       <c r="M82" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N82" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O82" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>274</v>
       </c>
@@ -5152,13 +4740,13 @@
       <c r="F83" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="K83" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L83" s="2" t="s">
@@ -5167,14 +4755,8 @@
       <c r="M83" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N83" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O83" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>275</v>
       </c>
@@ -5193,13 +4775,13 @@
       <c r="F84" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="K84" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L84" s="2" t="s">
@@ -5208,14 +4790,8 @@
       <c r="M84" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N84" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O84" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>276</v>
       </c>
@@ -5234,13 +4810,13 @@
       <c r="F85" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J85" s="2" t="s">
+      <c r="K85" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L85" s="2" t="s">
@@ -5249,14 +4825,8 @@
       <c r="M85" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O85" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>277</v>
       </c>
@@ -5275,13 +4845,13 @@
       <c r="F86" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J86" s="2" t="s">
+      <c r="K86" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L86" s="2" t="s">
@@ -5290,14 +4860,8 @@
       <c r="M86" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N86" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O86" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>278</v>
       </c>
@@ -5316,13 +4880,13 @@
       <c r="F87" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="K87" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L87" s="2" t="s">
@@ -5331,14 +4895,8 @@
       <c r="M87" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N87" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O87" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>279</v>
       </c>
@@ -5357,13 +4915,13 @@
       <c r="F88" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H88" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="K88" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L88" s="2" t="s">
@@ -5372,14 +4930,8 @@
       <c r="M88" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N88" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O88" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>280</v>
       </c>
@@ -5398,13 +4950,13 @@
       <c r="F89" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J89" s="2" t="s">
+      <c r="K89" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L89" s="2" t="s">
@@ -5413,14 +4965,8 @@
       <c r="M89" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O89" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>281</v>
       </c>
@@ -5439,13 +4985,13 @@
       <c r="F90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H90" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J90" s="2" t="s">
+      <c r="K90" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L90" s="2" t="s">
@@ -5454,14 +5000,8 @@
       <c r="M90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N90" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O90" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>282</v>
       </c>
@@ -5480,13 +5020,13 @@
       <c r="F91" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H91" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J91" s="2" t="s">
+      <c r="K91" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L91" s="2" t="s">
@@ -5495,14 +5035,8 @@
       <c r="M91" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O91" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>283</v>
       </c>
@@ -5521,13 +5055,13 @@
       <c r="F92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H92" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J92" s="2" t="s">
+      <c r="K92" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L92" s="2" t="s">
@@ -5536,14 +5070,8 @@
       <c r="M92" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O92" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>284</v>
       </c>
@@ -5562,13 +5090,13 @@
       <c r="F93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H93" s="2" t="s">
+      <c r="G93" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J93" s="2" t="s">
+      <c r="K93" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L93" s="2" t="s">
@@ -5577,14 +5105,8 @@
       <c r="M93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O93" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>285</v>
       </c>
@@ -5603,13 +5125,13 @@
       <c r="F94" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H94" s="2" t="s">
+      <c r="G94" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J94" s="2" t="s">
+      <c r="K94" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L94" s="2" t="s">
@@ -5618,14 +5140,8 @@
       <c r="M94" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O94" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>286</v>
       </c>
@@ -5644,13 +5160,13 @@
       <c r="F95" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="G95" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J95" s="2" t="s">
+      <c r="K95" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L95" s="2" t="s">
@@ -5659,14 +5175,8 @@
       <c r="M95" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O95" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>287</v>
       </c>
@@ -5685,13 +5195,13 @@
       <c r="F96" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J96" s="2" t="s">
+      <c r="K96" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L96" s="2" t="s">
@@ -5700,14 +5210,8 @@
       <c r="M96" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O96" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>288</v>
       </c>
@@ -5726,13 +5230,13 @@
       <c r="F97" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H97" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J97" s="2" t="s">
+      <c r="K97" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L97" s="2" t="s">
@@ -5741,14 +5245,8 @@
       <c r="M97" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O97" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>289</v>
       </c>
@@ -5767,13 +5265,13 @@
       <c r="F98" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J98" s="2" t="s">
+      <c r="K98" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L98" s="2" t="s">
@@ -5782,14 +5280,8 @@
       <c r="M98" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O98" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>290</v>
       </c>
@@ -5808,13 +5300,13 @@
       <c r="F99" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J99" s="2" t="s">
+      <c r="K99" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L99" s="2" t="s">
@@ -5823,14 +5315,8 @@
       <c r="M99" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N99" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O99" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>291</v>
       </c>
@@ -5849,13 +5335,13 @@
       <c r="F100" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J100" s="2" t="s">
+      <c r="K100" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L100" s="2" t="s">
@@ -5864,14 +5350,8 @@
       <c r="M100" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O100" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>329</v>
       </c>
@@ -5887,8 +5367,11 @@
       <c r="E101" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F101" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>225</v>
       </c>
@@ -5907,13 +5390,13 @@
       <c r="F102" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J102" s="2" t="s">
+      <c r="K102" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L102" s="2" t="s">
@@ -5922,14 +5405,8 @@
       <c r="M102" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O102" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>226</v>
       </c>
@@ -5948,13 +5425,13 @@
       <c r="F103" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H103" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J103" s="2" t="s">
+      <c r="K103" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L103" s="2" t="s">
@@ -5963,14 +5440,8 @@
       <c r="M103" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O103" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>227</v>
       </c>
@@ -5989,13 +5460,13 @@
       <c r="F104" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J104" s="2" t="s">
+      <c r="K104" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L104" s="2" t="s">
@@ -6004,14 +5475,8 @@
       <c r="M104" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O104" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>222</v>
       </c>
@@ -6030,13 +5495,13 @@
       <c r="F105" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H105" s="2" t="s">
+      <c r="G105" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J105" s="2" t="s">
+      <c r="K105" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L105" s="2" t="s">
@@ -6045,14 +5510,8 @@
       <c r="M105" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O105" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>223</v>
       </c>
@@ -6071,13 +5530,13 @@
       <c r="F106" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J106" s="2" t="s">
+      <c r="K106" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L106" s="2" t="s">
@@ -6086,14 +5545,8 @@
       <c r="M106" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O106" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>224</v>
       </c>
@@ -6112,13 +5565,13 @@
       <c r="F107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H107" s="2" t="s">
+      <c r="G107" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J107" s="2" t="s">
+      <c r="K107" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L107" s="2" t="s">
@@ -6127,14 +5580,8 @@
       <c r="M107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O107" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>228</v>
       </c>
@@ -6153,13 +5600,13 @@
       <c r="F108" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H108" s="2" t="s">
+      <c r="G108" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J108" s="2" t="s">
+      <c r="K108" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L108" s="2" t="s">
@@ -6168,14 +5615,8 @@
       <c r="M108" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O108" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>229</v>
       </c>
@@ -6194,13 +5635,13 @@
       <c r="F109" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H109" s="2" t="s">
+      <c r="G109" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J109" s="2" t="s">
+      <c r="K109" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L109" s="2" t="s">
@@ -6209,16 +5650,10 @@
       <c r="M109" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O109" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>247</v>
@@ -6235,13 +5670,13 @@
       <c r="F110" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H110" s="2" t="s">
+      <c r="G110" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J110" s="2" t="s">
+      <c r="K110" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L110" s="2" t="s">
@@ -6250,16 +5685,10 @@
       <c r="M110" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O110" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>250</v>
@@ -6276,13 +5705,13 @@
       <c r="F111" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H111" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J111" s="2" t="s">
+      <c r="K111" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L111" s="2" t="s">
@@ -6291,16 +5720,10 @@
       <c r="M111" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N111" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O111" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>252</v>
@@ -6317,13 +5740,13 @@
       <c r="F112" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="G112" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J112" s="2" t="s">
+      <c r="K112" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L112" s="2" t="s">
@@ -6332,16 +5755,10 @@
       <c r="M112" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O112" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>254</v>
@@ -6358,13 +5775,13 @@
       <c r="F113" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H113" s="2" t="s">
+      <c r="G113" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J113" s="2" t="s">
+      <c r="K113" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L113" s="2" t="s">
@@ -6373,16 +5790,10 @@
       <c r="M113" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N113" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O113" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>256</v>
@@ -6399,13 +5810,13 @@
       <c r="F114" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="G114" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J114" s="2" t="s">
+      <c r="K114" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L114" s="2" t="s">
@@ -6414,16 +5825,10 @@
       <c r="M114" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N114" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O114" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>346</v>
+        <v>258</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>259</v>
@@ -6440,13 +5845,13 @@
       <c r="F115" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H115" s="2" t="s">
+      <c r="G115" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J115" s="2" t="s">
+      <c r="K115" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L115" s="2" t="s">
@@ -6455,16 +5860,10 @@
       <c r="M115" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N115" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O115" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>309</v>
@@ -6481,13 +5880,13 @@
       <c r="F116" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H116" s="2" t="s">
+      <c r="G116" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J116" s="2" t="s">
+      <c r="K116" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L116" s="2" t="s">
@@ -6496,16 +5895,10 @@
       <c r="M116" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N116" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O116" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>292</v>
@@ -6522,13 +5915,13 @@
       <c r="F117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H117" s="2" t="s">
+      <c r="G117" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J117" s="2" t="s">
+      <c r="K117" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L117" s="2" t="s">
@@ -6537,16 +5930,10 @@
       <c r="M117" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O117" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>311</v>
@@ -6563,13 +5950,13 @@
       <c r="F118" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="G118" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J118" s="2" t="s">
+      <c r="K118" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L118" s="2" t="s">
@@ -6578,16 +5965,10 @@
       <c r="M118" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O118" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>313</v>
@@ -6604,13 +5985,13 @@
       <c r="F119" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J119" s="2" t="s">
+      <c r="K119" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L119" s="2" t="s">
@@ -6619,16 +6000,10 @@
       <c r="M119" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O119" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>331</v>
@@ -6645,13 +6020,13 @@
       <c r="F120" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="G120" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J120" s="2" t="s">
+      <c r="K120" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L120" s="2" t="s">
@@ -6660,16 +6035,10 @@
       <c r="M120" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O120" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>333</v>
@@ -6686,13 +6055,13 @@
       <c r="F121" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H121" s="2" t="s">
+      <c r="G121" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J121" s="2" t="s">
+      <c r="K121" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L121" s="2" t="s">
@@ -6701,186 +6070,217 @@
       <c r="M121" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N121" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O121" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>249</v>
       </c>
       <c r="E122" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E123" s="2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O121"/>
+  <autoFilter ref="A1:M121"/>
   <conditionalFormatting sqref="A110">
     <cfRule type="expression" dxfId="47" priority="41">
-      <formula>$R110="Passed"</formula>
+      <formula>$P110="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="46" priority="42">
-      <formula>$R110="Not Ready"</formula>
+      <formula>$P110="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="45" priority="43">
-      <formula>$R110="Retest"</formula>
+      <formula>$P110="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="44" priority="44">
-      <formula>$R110="Query"</formula>
+      <formula>$P110="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="43" priority="45">
-      <formula>$R110="Blocked"</formula>
+      <formula>$P110="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="42" priority="46">
-      <formula>$R110="In Progress"</formula>
+      <formula>$P110="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="41" priority="47">
-      <formula>$R110="N/A"</formula>
+      <formula>$P110="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="48">
-      <formula>$R110="Failed"</formula>
+      <formula>$P110="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111">
     <cfRule type="expression" dxfId="39" priority="33">
-      <formula>$R111="Passed"</formula>
+      <formula>$P111="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="38" priority="34">
-      <formula>$R111="Not Ready"</formula>
+      <formula>$P111="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="37" priority="35">
-      <formula>$R111="Retest"</formula>
+      <formula>$P111="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="36" priority="36">
-      <formula>$R111="Query"</formula>
+      <formula>$P111="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="35" priority="37">
-      <formula>$R111="Blocked"</formula>
+      <formula>$P111="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="38">
-      <formula>$R111="In Progress"</formula>
+      <formula>$P111="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="39">
-      <formula>$R111="N/A"</formula>
+      <formula>$P111="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="32" priority="40">
-      <formula>$R111="Failed"</formula>
+      <formula>$P111="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A112">
     <cfRule type="expression" dxfId="31" priority="25">
-      <formula>$R112="Passed"</formula>
+      <formula>$P112="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="30" priority="26">
-      <formula>$R112="Not Ready"</formula>
+      <formula>$P112="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="29" priority="27">
-      <formula>$R112="Retest"</formula>
+      <formula>$P112="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="28">
-      <formula>$R112="Query"</formula>
+      <formula>$P112="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="27" priority="29">
-      <formula>$R112="Blocked"</formula>
+      <formula>$P112="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="30">
-      <formula>$R112="In Progress"</formula>
+      <formula>$P112="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="31">
-      <formula>$R112="N/A"</formula>
+      <formula>$P112="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="24" priority="32">
-      <formula>$R112="Failed"</formula>
+      <formula>$P112="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114">
     <cfRule type="expression" dxfId="23" priority="17">
-      <formula>$R114="Passed"</formula>
+      <formula>$P114="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="18">
-      <formula>$R114="Not Ready"</formula>
+      <formula>$P114="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="19">
-      <formula>$R114="Retest"</formula>
+      <formula>$P114="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="20" priority="20">
-      <formula>$R114="Query"</formula>
+      <formula>$P114="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="21">
-      <formula>$R114="Blocked"</formula>
+      <formula>$P114="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="22">
-      <formula>$R114="In Progress"</formula>
+      <formula>$P114="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="17" priority="23">
-      <formula>$R114="N/A"</formula>
+      <formula>$P114="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="24">
-      <formula>$R114="Failed"</formula>
+      <formula>$P114="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A115">
     <cfRule type="expression" dxfId="15" priority="9">
-      <formula>$R115="Passed"</formula>
+      <formula>$P115="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="14" priority="10">
-      <formula>$R115="Not Ready"</formula>
+      <formula>$P115="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="11">
-      <formula>$R115="Retest"</formula>
+      <formula>$P115="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="12">
-      <formula>$R115="Query"</formula>
+      <formula>$P115="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="13">
-      <formula>$R115="Blocked"</formula>
+      <formula>$P115="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="14">
-      <formula>$R115="In Progress"</formula>
+      <formula>$P115="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="9" priority="15">
-      <formula>$R115="N/A"</formula>
+      <formula>$P115="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="16">
-      <formula>$R115="Failed"</formula>
+      <formula>$P115="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113">
     <cfRule type="expression" dxfId="7" priority="1">
-      <formula>$R113="Passed"</formula>
+      <formula>$P113="Passed"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$R113="Not Ready"</formula>
+      <formula>$P113="Not Ready"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="3">
-      <formula>$R113="Retest"</formula>
+      <formula>$P113="Retest"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="4">
-      <formula>$R113="Query"</formula>
+      <formula>$P113="Query"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="5">
-      <formula>$R113="Blocked"</formula>
+      <formula>$P113="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>$R113="In Progress"</formula>
+      <formula>$P113="In Progress"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="7">
-      <formula>$R113="N/A"</formula>
+      <formula>$P113="N/A"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>$R113="Failed"</formula>
+      <formula>$P113="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating Transfer Plan - Invoice On Account
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\BAU Aug 2021\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/674087_cognizant_com/Documents/Documents/WPP Global TestScripts/GlobalTestSuiteAutomation/WppRegpack/TestResource/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_D6735CE55F780992B22A6AFA6AEC16B7ACBB5D44" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BF10377-E7DF-48DF-BDBA-8079F65B57EB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalTestCase" sheetId="6" r:id="rId1"/>
@@ -33,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Cognizant</author>
   </authors>
   <commentList>
-    <comment ref="A23" authorId="0" shapeId="0">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B23" authorId="0" shapeId="0">
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C23" authorId="0" shapeId="0">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -111,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1400,7 +1401,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2248,11 +2249,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D154" sqref="D154"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,7 +3211,7 @@
         <v>114</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>128</v>
@@ -8190,7 +8191,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O152"/>
+  <autoFilter ref="A1:O152" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A121">
     <cfRule type="expression" dxfId="47" priority="41">
       <formula>$R121="Passed"</formula>
@@ -8354,7 +8355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10852,7 +10853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated TC Manager with latest TC names as per jira
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/TC_RunManager.xlsx
+++ b/WppRegpack/TestResource/TC_RunManager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuiteAutomation\WppRegpack\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuite\branches\bau_environment\WppRegpack\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32B83D9-6158-4AAF-80FB-38550F338293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60923E29-FF0D-42C5-B5DA-550D25F8843F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="420">
   <si>
     <t>Description</t>
   </si>
@@ -792,9 +792,6 @@
     <t>InvoicePlansDirectInvoice</t>
   </si>
   <si>
-    <t>Partial Invoicing Carry Forward</t>
-  </si>
-  <si>
     <t>PartialInvoicing_CarryForward</t>
   </si>
   <si>
@@ -819,9 +816,6 @@
     <t>Create_Blanket_Invoice</t>
   </si>
   <si>
-    <t>Customer Payment for Single Invoice</t>
-  </si>
-  <si>
     <t>Post a Customer Payment</t>
   </si>
   <si>
@@ -1405,6 +1399,18 @@
   </si>
   <si>
     <t>05. Fixed Assets Disposal</t>
+  </si>
+  <si>
+    <t>Customer Payment - Single Invoice</t>
+  </si>
+  <si>
+    <t>Invoicing Plans - Transfer Plan to Invoice On Account</t>
+  </si>
+  <si>
+    <t>Partial Invoicing, Write Off</t>
+  </si>
+  <si>
+    <t>Partial Invoicing, Carry Forward</t>
   </si>
 </sst>
 </file>
@@ -2521,8 +2527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,10 +2564,10 @@
         <v>118</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>87</v>
@@ -2576,7 +2582,7 @@
         <v>89</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>117</v>
@@ -2620,16 +2626,16 @@
         <v>6</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>6</v>
@@ -2667,13 +2673,13 @@
         <v>6</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>6</v>
@@ -2714,13 +2720,13 @@
         <v>6</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>6</v>
@@ -2761,13 +2767,13 @@
         <v>6</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>6</v>
@@ -2808,13 +2814,13 @@
         <v>6</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>6</v>
@@ -2855,13 +2861,13 @@
         <v>6</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>6</v>
@@ -2902,13 +2908,13 @@
         <v>6</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>6</v>
@@ -2949,13 +2955,13 @@
         <v>6</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>6</v>
@@ -2996,13 +3002,13 @@
         <v>6</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>6</v>
@@ -3043,13 +3049,13 @@
         <v>6</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>6</v>
@@ -3090,13 +3096,13 @@
         <v>6</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>6</v>
@@ -3137,13 +3143,13 @@
         <v>6</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>6</v>
@@ -3184,13 +3190,13 @@
         <v>6</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>6</v>
@@ -3231,13 +3237,13 @@
         <v>6</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>6</v>
@@ -3278,13 +3284,13 @@
         <v>6</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>6</v>
@@ -3325,13 +3331,13 @@
         <v>6</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>6</v>
@@ -3372,13 +3378,13 @@
         <v>6</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>6</v>
@@ -3419,13 +3425,13 @@
         <v>6</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>6</v>
@@ -3466,13 +3472,13 @@
         <v>6</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>6</v>
@@ -3513,13 +3519,13 @@
         <v>6</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>6</v>
@@ -3536,7 +3542,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>136</v>
+        <v>417</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>114</v>
@@ -3560,13 +3566,13 @@
         <v>6</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>6</v>
@@ -3610,7 +3616,7 @@
         <v>6</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -3639,13 +3645,13 @@
         <v>6</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>6</v>
@@ -3686,13 +3692,13 @@
         <v>6</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>6</v>
@@ -3733,13 +3739,13 @@
         <v>6</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>6</v>
@@ -3780,10 +3786,10 @@
         <v>6</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>6</v>
@@ -3824,10 +3830,10 @@
         <v>6</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>6</v>
@@ -3868,10 +3874,10 @@
         <v>6</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>6</v>
@@ -3912,10 +3918,10 @@
         <v>6</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>6</v>
@@ -3956,10 +3962,10 @@
         <v>6</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>6</v>
@@ -4001,10 +4007,10 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>6</v>
@@ -4046,10 +4052,10 @@
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>6</v>
@@ -4091,10 +4097,10 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>6</v>
@@ -4135,10 +4141,10 @@
         <v>6</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>6</v>
@@ -4179,10 +4185,10 @@
         <v>6</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>6</v>
@@ -4214,10 +4220,10 @@
         <v>6</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>6</v>
@@ -4249,10 +4255,10 @@
         <v>6</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>6</v>
@@ -4293,10 +4299,10 @@
         <v>6</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>6</v>
@@ -4328,10 +4334,10 @@
         <v>6</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>6</v>
@@ -4363,10 +4369,10 @@
         <v>6</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>6</v>
@@ -4407,10 +4413,10 @@
         <v>6</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>6</v>
@@ -4442,10 +4448,10 @@
         <v>6</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>6</v>
@@ -4477,13 +4483,13 @@
         <v>6</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -4512,10 +4518,10 @@
         <v>6</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -4544,15 +4550,15 @@
         <v>6</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>139</v>
+        <v>418</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>131</v>
@@ -4579,18 +4585,18 @@
         <v>6</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>128</v>
@@ -4611,7 +4617,7 @@
         <v>6</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>6</v>
@@ -4655,7 +4661,7 @@
         <v>6</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>6</v>
@@ -4672,13 +4678,13 @@
     </row>
     <row r="50" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>218</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>128</v>
@@ -4697,10 +4703,10 @@
       </c>
       <c r="I50" s="11"/>
       <c r="J50" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>6</v>
@@ -4717,13 +4723,13 @@
     </row>
     <row r="51" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="C51" s="10" t="s">
         <v>220</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>221</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>128</v>
@@ -4742,10 +4748,10 @@
       </c>
       <c r="I51" s="11"/>
       <c r="J51" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>6</v>
@@ -4762,7 +4768,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>222</v>
+        <v>416</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>51</v>
@@ -4786,13 +4792,13 @@
         <v>6</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>6</v>
@@ -4809,7 +4815,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>49</v>
@@ -4833,13 +4839,13 @@
         <v>6</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>6</v>
@@ -4856,13 +4862,13 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>124</v>
@@ -4880,10 +4886,10 @@
         <v>6</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>6</v>
@@ -4900,13 +4906,13 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>124</v>
@@ -4924,10 +4930,10 @@
         <v>6</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>6</v>
@@ -4944,13 +4950,13 @@
     </row>
     <row r="56" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>230</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>232</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>128</v>
@@ -4969,10 +4975,10 @@
       </c>
       <c r="I56" s="11"/>
       <c r="J56" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>6</v>
@@ -4989,7 +4995,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>53</v>
@@ -5013,13 +5019,13 @@
         <v>6</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>6</v>
@@ -5036,7 +5042,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>106</v>
@@ -5060,13 +5066,13 @@
         <v>6</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>6</v>
@@ -5083,13 +5089,13 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>127</v>
@@ -5107,13 +5113,13 @@
         <v>6</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>6</v>
@@ -5130,7 +5136,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>108</v>
@@ -5154,13 +5160,13 @@
         <v>6</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L60" s="2" t="s">
         <v>6</v>
@@ -5177,10 +5183,10 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>107</v>
@@ -5201,13 +5207,13 @@
         <v>6</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>6</v>
@@ -5224,13 +5230,13 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>127</v>
@@ -5248,13 +5254,13 @@
         <v>6</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>6</v>
@@ -5271,7 +5277,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>111</v>
@@ -5295,13 +5301,13 @@
         <v>6</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>6</v>
@@ -5318,13 +5324,13 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>127</v>
@@ -5342,13 +5348,13 @@
         <v>6</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>6</v>
@@ -5356,13 +5362,13 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>121</v>
@@ -5380,10 +5386,10 @@
         <v>6</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>6</v>
@@ -5400,17 +5406,17 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="D66" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="E66" s="2" t="s">
         <v>6</v>
       </c>
@@ -5424,10 +5430,10 @@
         <v>6</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>2</v>
@@ -5447,16 +5453,16 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="D67" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>6</v>
@@ -5471,13 +5477,13 @@
         <v>6</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>6</v>
@@ -5494,16 +5500,16 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>6</v>
@@ -5518,13 +5524,13 @@
         <v>6</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>6</v>
@@ -5541,16 +5547,16 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>260</v>
-      </c>
       <c r="D69" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>6</v>
@@ -5565,13 +5571,13 @@
         <v>6</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>6</v>
@@ -5588,16 +5594,16 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="C70" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>6</v>
@@ -5615,22 +5621,22 @@
         <v>6</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="E71" s="2" t="s">
         <v>6</v>
       </c>
@@ -5647,7 +5653,7 @@
         <v>6</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>6</v>
@@ -5664,16 +5670,16 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>6</v>
@@ -5691,7 +5697,7 @@
         <v>6</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>6</v>
@@ -5708,16 +5714,16 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>260</v>
-      </c>
       <c r="D73" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>6</v>
@@ -5735,7 +5741,7 @@
         <v>6</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>6</v>
@@ -5752,16 +5758,16 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="D74" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>6</v>
@@ -5779,21 +5785,21 @@
         <v>6</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="D75" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>6</v>
@@ -5808,13 +5814,13 @@
         <v>6</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L75" s="2" t="s">
         <v>6</v>
@@ -5831,16 +5837,16 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>6</v>
@@ -5855,45 +5861,45 @@
         <v>6</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K77" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>6</v>
@@ -5901,7 +5907,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>17</v>
@@ -5910,7 +5916,7 @@
         <v>18</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>6</v>
@@ -5928,7 +5934,7 @@
         <v>6</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>6</v>
@@ -5945,7 +5951,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>15</v>
@@ -5954,7 +5960,7 @@
         <v>16</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>6</v>
@@ -5972,7 +5978,7 @@
         <v>6</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>6</v>
@@ -5989,7 +5995,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>20</v>
@@ -5998,7 +6004,7 @@
         <v>20</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>6</v>
@@ -6016,7 +6022,7 @@
         <v>6</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>6</v>
@@ -6033,16 +6039,16 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>6</v>
@@ -6060,7 +6066,7 @@
         <v>6</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>6</v>
@@ -6077,16 +6083,16 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>6</v>
@@ -6104,7 +6110,7 @@
         <v>6</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L82" s="2" t="s">
         <v>6</v>
@@ -6121,16 +6127,16 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>6</v>
@@ -6148,7 +6154,7 @@
         <v>6</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>6</v>
@@ -6165,7 +6171,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>99</v>
@@ -6192,7 +6198,7 @@
         <v>6</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>6</v>
@@ -6209,7 +6215,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>100</v>
@@ -6236,7 +6242,7 @@
         <v>6</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>6</v>
@@ -6253,7 +6259,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>94</v>
@@ -6280,7 +6286,7 @@
         <v>6</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L86" s="2" t="s">
         <v>6</v>
@@ -6297,7 +6303,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>92</v>
@@ -6324,7 +6330,7 @@
         <v>6</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L87" s="2" t="s">
         <v>6</v>
@@ -6341,13 +6347,13 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>119</v>
@@ -6368,7 +6374,7 @@
         <v>6</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>6</v>
@@ -6385,7 +6391,7 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>84</v>
@@ -6412,7 +6418,7 @@
         <v>6</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>6</v>
@@ -6429,7 +6435,7 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>85</v>
@@ -6456,7 +6462,7 @@
         <v>6</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L90" s="2" t="s">
         <v>6</v>
@@ -6473,7 +6479,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>101</v>
@@ -6500,7 +6506,7 @@
         <v>6</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>6</v>
@@ -6517,7 +6523,7 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>97</v>
@@ -6544,7 +6550,7 @@
         <v>6</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>6</v>
@@ -6561,7 +6567,7 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>96</v>
@@ -6588,7 +6594,7 @@
         <v>6</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>6</v>
@@ -6605,13 +6611,13 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>283</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>119</v>
@@ -6632,7 +6638,7 @@
         <v>6</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>6</v>
@@ -6649,7 +6655,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>79</v>
@@ -6676,7 +6682,7 @@
         <v>6</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>6</v>
@@ -6693,7 +6699,7 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>75</v>
@@ -6720,7 +6726,7 @@
         <v>6</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>6</v>
@@ -6737,7 +6743,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>77</v>
@@ -6764,7 +6770,7 @@
         <v>6</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>6</v>
@@ -6781,7 +6787,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>81</v>
@@ -6808,7 +6814,7 @@
         <v>6</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>6</v>
@@ -6825,7 +6831,7 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>71</v>
@@ -6852,7 +6858,7 @@
         <v>6</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>6</v>
@@ -6869,7 +6875,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>70</v>
@@ -6896,7 +6902,7 @@
         <v>6</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>6</v>
@@ -6913,7 +6919,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>102</v>
@@ -6940,7 +6946,7 @@
         <v>6</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>6</v>
@@ -6957,13 +6963,13 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>154</v>
@@ -6984,7 +6990,7 @@
         <v>6</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>6</v>
@@ -7001,13 +7007,13 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>291</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>154</v>
@@ -7028,7 +7034,7 @@
         <v>6</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>6</v>
@@ -7045,7 +7051,7 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>83</v>
@@ -7072,7 +7078,7 @@
         <v>6</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L104" s="2" t="s">
         <v>6</v>
@@ -7089,7 +7095,7 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>74</v>
@@ -7116,7 +7122,7 @@
         <v>6</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L105" s="2" t="s">
         <v>6</v>
@@ -7133,7 +7139,7 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>143</v>
@@ -7160,7 +7166,7 @@
         <v>6</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>6</v>
@@ -7177,7 +7183,7 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>147</v>
@@ -7204,7 +7210,7 @@
         <v>6</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>6</v>
@@ -7221,7 +7227,7 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>145</v>
@@ -7248,7 +7254,7 @@
         <v>6</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>6</v>
@@ -7265,7 +7271,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>146</v>
@@ -7292,7 +7298,7 @@
         <v>6</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L109" s="2" t="s">
         <v>6</v>
@@ -7309,7 +7315,7 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>148</v>
@@ -7336,7 +7342,7 @@
         <v>6</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L110" s="2" t="s">
         <v>6</v>
@@ -7353,13 +7359,13 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>144</v>
@@ -7380,7 +7386,7 @@
         <v>6</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>6</v>
@@ -7397,13 +7403,13 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>144</v>
@@ -7424,7 +7430,7 @@
         <v>6</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>6</v>
@@ -7432,16 +7438,16 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D113" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>6</v>
@@ -7473,7 +7479,7 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>47</v>
@@ -7497,10 +7503,10 @@
         <v>6</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>6</v>
@@ -7517,7 +7523,7 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>33</v>
@@ -7544,7 +7550,7 @@
         <v>6</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L115" s="2" t="s">
         <v>6</v>
@@ -7561,7 +7567,7 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>45</v>
@@ -7588,7 +7594,7 @@
         <v>6</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L116" s="2" t="s">
         <v>6</v>
@@ -7605,13 +7611,13 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>125</v>
@@ -7632,7 +7638,7 @@
         <v>6</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L117" s="2" t="s">
         <v>6</v>
@@ -7649,13 +7655,13 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>125</v>
@@ -7676,7 +7682,7 @@
         <v>6</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L118" s="2" t="s">
         <v>6</v>
@@ -7693,7 +7699,7 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>110</v>
@@ -7720,7 +7726,7 @@
         <v>6</v>
       </c>
       <c r="K119" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L119" s="2" t="s">
         <v>6</v>
@@ -7764,7 +7770,7 @@
         <v>6</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>6</v>
@@ -7781,17 +7787,17 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>307</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="D121" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="E121" s="2" t="s">
         <v>6</v>
       </c>
@@ -7808,7 +7814,7 @@
         <v>6</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>6</v>
@@ -7825,16 +7831,16 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>311</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="D122" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>6</v>
@@ -7852,7 +7858,7 @@
         <v>6</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L122" s="2" t="s">
         <v>6</v>
@@ -7869,16 +7875,16 @@
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>314</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="D123" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>6</v>
@@ -7896,7 +7902,7 @@
         <v>6</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L123" s="2" t="s">
         <v>6</v>
@@ -7913,16 +7919,16 @@
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>317</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="D124" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>2</v>
@@ -7940,7 +7946,7 @@
         <v>6</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>6</v>
@@ -7957,16 +7963,16 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>320</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B125" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="D125" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>6</v>
@@ -7984,7 +7990,7 @@
         <v>6</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>6</v>
@@ -8001,16 +8007,16 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>6</v>
@@ -8028,7 +8034,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>6</v>
@@ -8045,16 +8051,16 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>325</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="D127" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>6</v>
@@ -8072,7 +8078,7 @@
         <v>6</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L127" s="2" t="s">
         <v>6</v>
@@ -8089,16 +8095,16 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>6</v>
@@ -8116,7 +8122,7 @@
         <v>6</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>6</v>
@@ -8133,16 +8139,16 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>330</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>334</v>
-      </c>
       <c r="D129" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>6</v>
@@ -8160,7 +8166,7 @@
         <v>6</v>
       </c>
       <c r="K129" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L129" s="2" t="s">
         <v>6</v>
@@ -8177,16 +8183,16 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>333</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="D130" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>6</v>
@@ -8204,7 +8210,7 @@
         <v>6</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>6</v>
@@ -8221,16 +8227,16 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>340</v>
-      </c>
       <c r="D131" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>6</v>
@@ -8248,7 +8254,7 @@
         <v>6</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>6</v>
@@ -8265,16 +8271,16 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>343</v>
-      </c>
       <c r="D132" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>6</v>
@@ -8292,7 +8298,7 @@
         <v>6</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>6</v>
@@ -8309,16 +8315,16 @@
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="D133" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>6</v>
@@ -8344,16 +8350,16 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="D134" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>6</v>
@@ -8368,10 +8374,10 @@
         <v>6</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K134" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L134" s="2" t="s">
         <v>6</v>
@@ -8379,16 +8385,16 @@
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>6</v>
@@ -8403,10 +8409,10 @@
         <v>6</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L135" s="2" t="s">
         <v>6</v>
@@ -8414,16 +8420,16 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>6</v>
@@ -8446,16 +8452,16 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="C137" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D137" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>6</v>
@@ -8478,16 +8484,16 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>6</v>
@@ -8510,16 +8516,16 @@
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>6</v>
@@ -8537,16 +8543,16 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>158</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>6</v>
@@ -8564,16 +8570,16 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>6</v>
@@ -8591,16 +8597,16 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>162</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>6</v>
@@ -8618,16 +8624,16 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>6</v>
@@ -8648,7 +8654,7 @@
         <v>6</v>
       </c>
       <c r="L143" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M143" s="2" t="s">
         <v>6</v>
@@ -8665,16 +8671,16 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>6</v>
@@ -8695,7 +8701,7 @@
         <v>6</v>
       </c>
       <c r="L144" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M144" s="2" t="s">
         <v>6</v>
@@ -8712,16 +8718,16 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>172</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>6</v>
@@ -8742,7 +8748,7 @@
         <v>6</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M145" s="2" t="s">
         <v>6</v>
@@ -8759,16 +8765,16 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>6</v>
@@ -8789,7 +8795,7 @@
         <v>6</v>
       </c>
       <c r="L146" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M146" s="2" t="s">
         <v>6</v>
@@ -8806,16 +8812,16 @@
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>6</v>
@@ -8836,7 +8842,7 @@
         <v>6</v>
       </c>
       <c r="L147" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M147" s="2" t="s">
         <v>6</v>
@@ -8853,16 +8859,16 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>6</v>
@@ -8881,7 +8887,7 @@
         <v>6</v>
       </c>
       <c r="L148" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M148" s="2" t="s">
         <v>6</v>
@@ -8889,16 +8895,16 @@
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>6</v>
@@ -8916,16 +8922,16 @@
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>6</v>
@@ -8943,13 +8949,13 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>121</v>
@@ -8967,18 +8973,18 @@
         <v>6</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>121</v>
@@ -8987,21 +8993,21 @@
         <v>6</v>
       </c>
       <c r="K152" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>397</v>
-      </c>
       <c r="D153" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J153" s="2" t="s">
         <v>2</v>

</xml_diff>